<commit_message>
Model Results xlx updated
</commit_message>
<xml_diff>
--- a/Models Statistics.xlsx
+++ b/Models Statistics.xlsx
@@ -1,13 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minus\Documents\GitHub\Deep-Learning-Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
-    <sheet name="First Go Model(cleaned data)" sheetId="2" r:id="rId1"/>
+    <sheet name="FFN (clean data)" sheetId="2" r:id="rId1"/>
     <sheet name="Second Model" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="31">
   <si>
     <t>max_length</t>
   </si>
@@ -42,17 +47,80 @@
     <t>(baseline)</t>
   </si>
   <si>
-    <t>(Baseline)</t>
-  </si>
-  <si>
     <t>Notes: Lines with Green color have better results from the previous and Red colour lines have worse</t>
+  </si>
+  <si>
+    <t>Level 1 Neurons</t>
+  </si>
+  <si>
+    <t>Level 2 Neurons</t>
+  </si>
+  <si>
+    <t>validation_split</t>
+  </si>
+  <si>
+    <t>optimizer</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>sgd</t>
+  </si>
+  <si>
+    <t>RMSprop</t>
+  </si>
+  <si>
+    <t>Adagrad</t>
+  </si>
+  <si>
+    <t>l2=0.01</t>
+  </si>
+  <si>
+    <t>regularization</t>
+  </si>
+  <si>
+    <t>dropout = 0.2</t>
+  </si>
+  <si>
+    <t>no dropout</t>
+  </si>
+  <si>
+    <t>tokenization</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>tfidf</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>Non IT Jobs (cleaned)</t>
+  </si>
+  <si>
+    <t>2nd Layer Activation</t>
+  </si>
+  <si>
+    <t>tanh</t>
+  </si>
+  <si>
+    <t>relu</t>
+  </si>
+  <si>
+    <t>random_state = 17, test_size = 0.1</t>
+  </si>
+  <si>
+    <t>tanh (1st)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,13 +132,6 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,6 +166,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -132,29 +228,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -165,6 +273,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -213,7 +324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,7 +359,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -457,135 +568,1208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="8" customWidth="1"/>
+    <col min="5" max="6" width="16.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="E1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>0.63</v>
       </c>
-      <c r="B2" s="3">
-        <v>1000</v>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="9">
+        <v>30</v>
+      </c>
+      <c r="D2" s="9">
+        <v>200</v>
+      </c>
+      <c r="E2" s="8">
+        <v>512</v>
+      </c>
+      <c r="F2" s="8">
+        <v>512</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>0.62</v>
+      </c>
+      <c r="B3" s="10">
+        <v>500</v>
+      </c>
+      <c r="C3" s="10">
+        <v>30</v>
+      </c>
+      <c r="D3" s="10">
+        <v>200</v>
+      </c>
+      <c r="E3" s="8">
+        <v>512</v>
+      </c>
+      <c r="F3" s="8">
+        <v>512</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>0.61</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="10">
+        <v>30</v>
+      </c>
+      <c r="D4" s="10">
+        <v>100</v>
+      </c>
+      <c r="E4" s="8">
+        <v>512</v>
+      </c>
+      <c r="F4" s="8">
+        <v>512</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="11">
+        <v>30</v>
+      </c>
+      <c r="D5" s="11">
+        <v>400</v>
+      </c>
+      <c r="E5" s="8">
+        <v>512</v>
+      </c>
+      <c r="F5" s="8">
+        <v>512</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>0.62</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="10">
+        <v>30</v>
+      </c>
+      <c r="D6" s="10">
+        <v>500</v>
+      </c>
+      <c r="E6" s="8">
+        <v>512</v>
+      </c>
+      <c r="F6" s="8">
+        <v>512</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C13" s="8">
+        <v>100</v>
+      </c>
+      <c r="D13" s="8">
+        <v>32</v>
+      </c>
+      <c r="E13" s="8">
+        <v>512</v>
+      </c>
+      <c r="F13" s="8">
+        <v>512</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="B14" s="8">
+        <v>500</v>
+      </c>
+      <c r="C14" s="8">
+        <v>100</v>
+      </c>
+      <c r="D14" s="8">
+        <v>32</v>
+      </c>
+      <c r="E14" s="8">
+        <v>512</v>
+      </c>
+      <c r="F14" s="8">
+        <v>512</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="B15" s="8">
+        <v>500</v>
+      </c>
+      <c r="C15" s="8">
+        <v>100</v>
+      </c>
+      <c r="D15" s="8">
+        <v>16</v>
+      </c>
+      <c r="E15" s="8">
+        <v>512</v>
+      </c>
+      <c r="F15" s="8">
+        <v>512</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="B16" s="8">
+        <v>500</v>
+      </c>
+      <c r="C16" s="8">
+        <v>50</v>
+      </c>
+      <c r="D16" s="8">
+        <v>16</v>
+      </c>
+      <c r="E16" s="8">
+        <v>512</v>
+      </c>
+      <c r="F16" s="8">
+        <v>512</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="B17" s="8">
+        <v>500</v>
+      </c>
+      <c r="C17" s="8">
+        <v>50</v>
+      </c>
+      <c r="D17" s="8">
+        <v>64</v>
+      </c>
+      <c r="E17" s="8">
+        <v>512</v>
+      </c>
+      <c r="F17" s="8">
+        <v>512</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="B18" s="8">
+        <v>5000</v>
+      </c>
+      <c r="C18" s="8">
+        <v>50</v>
+      </c>
+      <c r="D18" s="8">
+        <v>64</v>
+      </c>
+      <c r="E18" s="8">
+        <v>512</v>
+      </c>
+      <c r="F18" s="8">
+        <v>512</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="B19" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C19" s="13">
+        <v>50</v>
+      </c>
+      <c r="D19" s="13">
+        <v>64</v>
+      </c>
+      <c r="E19" s="13">
+        <v>1024</v>
+      </c>
+      <c r="F19" s="13">
+        <v>512</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C20" s="8">
+        <v>50</v>
+      </c>
+      <c r="D20" s="8">
+        <v>64</v>
+      </c>
+      <c r="E20" s="8">
+        <v>2048</v>
+      </c>
+      <c r="F20" s="8">
+        <v>1024</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C21" s="8">
+        <v>50</v>
+      </c>
+      <c r="D21" s="8">
+        <v>64</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1024</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1024</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="B22" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="13">
+        <v>50</v>
+      </c>
+      <c r="D22" s="13">
+        <v>64</v>
+      </c>
+      <c r="E22" s="13">
+        <v>1024</v>
+      </c>
+      <c r="F22" s="13">
+        <v>512</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="B23" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C23" s="13">
+        <v>50</v>
+      </c>
+      <c r="D23" s="13">
+        <v>32</v>
+      </c>
+      <c r="E23" s="13">
+        <v>1024</v>
+      </c>
+      <c r="F23" s="13">
+        <v>512</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="B24" s="12">
+        <v>1000</v>
+      </c>
+      <c r="C24" s="12">
+        <v>50</v>
+      </c>
+      <c r="D24" s="12">
+        <v>32</v>
+      </c>
+      <c r="E24" s="12">
+        <v>1024</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="B25" s="12">
+        <v>1000</v>
+      </c>
+      <c r="C25" s="12">
+        <v>50</v>
+      </c>
+      <c r="D25" s="12">
+        <v>32</v>
+      </c>
+      <c r="E25" s="12">
+        <v>2048</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="B26" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C26" s="13">
+        <v>50</v>
+      </c>
+      <c r="D26" s="13">
+        <v>32</v>
+      </c>
+      <c r="E26" s="13">
+        <v>4096</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="B27" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C27" s="13">
+        <v>50</v>
+      </c>
+      <c r="D27" s="13">
+        <v>32</v>
+      </c>
+      <c r="E27" s="13">
+        <v>2048</v>
+      </c>
+      <c r="F27" s="13">
+        <v>512</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="B28" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C28" s="13">
+        <v>50</v>
+      </c>
+      <c r="D28" s="13">
+        <v>32</v>
+      </c>
+      <c r="E28" s="13">
+        <v>2048</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="B29" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C29" s="13">
+        <v>50</v>
+      </c>
+      <c r="D29" s="13">
+        <v>32</v>
+      </c>
+      <c r="E29" s="13">
+        <v>2048</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="B30" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C30" s="13">
+        <v>50</v>
+      </c>
+      <c r="D30" s="13">
+        <v>32</v>
+      </c>
+      <c r="E30" s="13">
+        <v>2048</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="B31" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C31" s="13">
+        <v>50</v>
+      </c>
+      <c r="D31" s="13">
+        <v>32</v>
+      </c>
+      <c r="E31" s="13">
+        <v>2048</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="B32" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C32" s="8">
+        <v>50</v>
+      </c>
+      <c r="D32" s="8">
+        <v>32</v>
+      </c>
+      <c r="E32" s="8">
+        <v>2048</v>
+      </c>
+      <c r="F32" s="8">
+        <v>4096</v>
+      </c>
+      <c r="G32" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>0.62</v>
+      </c>
+      <c r="B33" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C33" s="8">
+        <v>50</v>
+      </c>
+      <c r="D33" s="8">
+        <v>32</v>
+      </c>
+      <c r="E33" s="8">
+        <v>2048</v>
+      </c>
+      <c r="F33" s="8">
+        <v>1024</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="B34" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C34" s="8">
+        <v>50</v>
+      </c>
+      <c r="D34" s="8">
+        <v>32</v>
+      </c>
+      <c r="E34" s="8">
+        <v>2048</v>
+      </c>
+      <c r="F34" s="8">
+        <v>1024</v>
+      </c>
+      <c r="G34" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="12">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="B35" s="12">
+        <v>1000</v>
+      </c>
+      <c r="C35" s="12">
+        <v>50</v>
+      </c>
+      <c r="D35" s="12">
+        <v>32</v>
+      </c>
+      <c r="E35" s="12">
+        <v>2048</v>
+      </c>
+      <c r="F35" s="12">
+        <v>1024</v>
+      </c>
+      <c r="G35" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="B36" s="12">
+        <v>1000</v>
+      </c>
+      <c r="C36" s="12">
+        <v>50</v>
+      </c>
+      <c r="D36" s="12">
+        <v>32</v>
+      </c>
+      <c r="E36" s="12">
+        <v>2048</v>
+      </c>
+      <c r="F36" s="12">
+        <v>1024</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="B37" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C37" s="13">
+        <v>100</v>
+      </c>
+      <c r="D37" s="13">
+        <v>32</v>
+      </c>
+      <c r="E37" s="13">
+        <v>2048</v>
+      </c>
+      <c r="F37" s="13">
+        <v>1024</v>
+      </c>
+      <c r="G37" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="B38" s="8">
+        <v>1000</v>
+      </c>
+      <c r="C38" s="8">
+        <v>50</v>
+      </c>
+      <c r="D38" s="8">
+        <v>32</v>
+      </c>
+      <c r="E38" s="8">
+        <v>2048</v>
+      </c>
+      <c r="G38" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3">
-        <v>30</v>
-      </c>
-      <c r="E2" s="3">
-        <v>200</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>0.62</v>
-      </c>
-      <c r="B3" s="8">
-        <v>500</v>
-      </c>
-      <c r="C3" s="8">
-        <v>25</v>
-      </c>
-      <c r="D3" s="8">
-        <v>30</v>
-      </c>
-      <c r="E3" s="8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>0.61</v>
-      </c>
-      <c r="B4" s="8">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="8">
-        <v>25</v>
-      </c>
-      <c r="D4" s="8">
-        <v>30</v>
-      </c>
-      <c r="E4" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>0.63</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1000</v>
-      </c>
-      <c r="C5" s="5">
-        <v>25</v>
-      </c>
-      <c r="D5" s="5">
-        <v>30</v>
-      </c>
-      <c r="E5" s="5">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>0.62</v>
-      </c>
-      <c r="B6" s="8">
-        <v>1000</v>
-      </c>
-      <c r="C6" s="8">
-        <v>25</v>
-      </c>
-      <c r="D6" s="8">
-        <v>30</v>
-      </c>
-      <c r="E6" s="8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="13">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="B42" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C42" s="13">
+        <v>50</v>
+      </c>
+      <c r="D42" s="13">
+        <v>64</v>
+      </c>
+      <c r="E42" s="13">
+        <v>1024</v>
+      </c>
+      <c r="F42" s="13">
+        <v>512</v>
+      </c>
+      <c r="G42" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="13">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="B43" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C43" s="13">
+        <v>50</v>
+      </c>
+      <c r="D43" s="13">
+        <v>32</v>
+      </c>
+      <c r="E43" s="13">
+        <v>1024</v>
+      </c>
+      <c r="F43" s="13">
+        <v>512</v>
+      </c>
+      <c r="G43" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="12">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="B44" s="12">
+        <v>1000</v>
+      </c>
+      <c r="C44" s="12">
+        <v>50</v>
+      </c>
+      <c r="D44" s="12">
+        <v>32</v>
+      </c>
+      <c r="E44" s="12">
+        <v>1024</v>
+      </c>
+      <c r="F44" s="12">
+        <v>512</v>
+      </c>
+      <c r="G44" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="B45" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C45" s="13">
+        <v>50</v>
+      </c>
+      <c r="D45" s="13">
+        <v>32</v>
+      </c>
+      <c r="E45" s="13">
+        <v>1024</v>
+      </c>
+      <c r="F45" s="13">
+        <v>512</v>
+      </c>
+      <c r="G45" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="B46" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C46" s="13">
+        <v>50</v>
+      </c>
+      <c r="D46" s="13">
+        <v>32</v>
+      </c>
+      <c r="E46" s="13">
+        <v>1024</v>
+      </c>
+      <c r="F46" s="13">
+        <v>512</v>
+      </c>
+      <c r="G46" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="B47" s="13">
+        <v>1000</v>
+      </c>
+      <c r="C47" s="13">
+        <v>50</v>
+      </c>
+      <c r="D47" s="13">
+        <v>32</v>
+      </c>
+      <c r="E47" s="13">
+        <v>2048</v>
+      </c>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A41:H41"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -633,25 +1817,25 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>0.31</v>
       </c>
-      <c r="B2" s="7">
-        <v>1000</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="B2" s="6">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="6">
         <v>25</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>15</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>30</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -659,100 +1843,100 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>0.34</v>
       </c>
-      <c r="B3" s="5">
-        <v>1000</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="B3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="4">
         <v>25</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>15</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>30</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>0.35</v>
       </c>
-      <c r="B4" s="5">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="4">
         <v>500</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>25</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>15</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>30</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>0.37</v>
       </c>
-      <c r="B5" s="5">
-        <v>1000</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="4">
         <v>500</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>25</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>20</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>30</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>0.38</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>500</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>500</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>25</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>20</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>30</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CNN Testing + Small fixes
</commit_message>
<xml_diff>
--- a/Models Statistics.xlsx
+++ b/Models Statistics.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FFN (clean data)" sheetId="2" r:id="rId1"/>
     <sheet name="Second Model" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="CNN (clean data)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="38">
   <si>
     <t>max_length</t>
   </si>
@@ -114,12 +114,37 @@
   </si>
   <si>
     <t>tanh (1st)</t>
+  </si>
+  <si>
+    <t>Embedding Dims</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sequences length </t>
+  </si>
+  <si>
+    <t>CNN filters</t>
+  </si>
+  <si>
+    <t>kernel size</t>
+  </si>
+  <si>
+    <t>Dense Layer dims</t>
+  </si>
+  <si>
+    <t>Dense Activation</t>
+  </si>
+  <si>
+    <t>Dense Dropout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -264,6 +289,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1947,12 +1976,284 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" s="16" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="B6" s="16">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1200</v>
+      </c>
+      <c r="D6" s="16">
+        <v>32</v>
+      </c>
+      <c r="E6" s="16">
+        <v>64</v>
+      </c>
+      <c r="F6" s="17">
+        <v>10</v>
+      </c>
+      <c r="G6" s="17">
+        <v>100</v>
+      </c>
+      <c r="H6" s="17">
+        <v>16</v>
+      </c>
+      <c r="I6" s="17">
+        <v>50</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0</v>
+      </c>
+      <c r="L6" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>0.64</v>
+      </c>
+      <c r="B7" s="16">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="16">
+        <v>1200</v>
+      </c>
+      <c r="D7" s="16">
+        <v>32</v>
+      </c>
+      <c r="E7" s="16">
+        <v>64</v>
+      </c>
+      <c r="F7" s="17">
+        <v>20</v>
+      </c>
+      <c r="G7" s="17">
+        <v>100</v>
+      </c>
+      <c r="H7" s="17">
+        <v>16</v>
+      </c>
+      <c r="I7" s="17">
+        <v>50</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0</v>
+      </c>
+      <c r="L7" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>